<commit_message>
Expanded template spreadsheet for sessions
</commit_message>
<xml_diff>
--- a/_data/sessions.xlsx
+++ b/_data/sessions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Github/jirelations/23digitale/_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Github/jirelations/23rw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D23F0ADE-6D0D-BE40-BF96-4BBEA214FB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767224BE-0A16-F94A-899C-093AAB6DFB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F7F6A8B1-B433-1145-8F64-4C3194B5E823}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{F7F6A8B1-B433-1145-8F64-4C3194B5E823}"/>
   </bookViews>
   <sheets>
     <sheet name="sessions" sheetId="1" r:id="rId1"/>
@@ -36,11 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
   <si>
     <t>session</t>
   </si>
   <si>
+    <t>contents</t>
+  </si>
+  <si>
     <t>title</t>
   </si>
   <si>
@@ -57,12 +66,28 @@
   </si>
   <si>
     <t>objective</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>zotero-readings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="dd\.mm"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -100,9 +125,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,68 +408,618 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21747042-CCAC-104E-9F8E-130EDA7419B3}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="31.83203125" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="3"/>
+      <c r="D2" s="2">
+        <f>IF(LEN(C2),TEXT(C2, "YYYY-MM-DD") &amp; "-" &amp; B2 &amp; ".md",)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" t="str">
+        <f>B2 &amp; ". " &amp; F2</f>
+        <v xml:space="preserve">1. </v>
+      </c>
+      <c r="H2">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(G2,".",""),"&amp;","")," ","-"),"--","-")</f>
+        <v>1-</v>
+      </c>
+      <c r="M2" t="str">
+        <f>"["&amp;B2&amp;"]"</f>
+        <v>[1]</v>
+      </c>
+      <c r="N2" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B2 &amp; "
+" &amp; M$1 &amp; ": " &amp; M2 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 1
+tags: [1]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="3"/>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D12" si="0">IF(LEN(C3),TEXT(C3, "YYYY-MM-DD") &amp; "-" &amp; B3 &amp; ".md",)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G12" si="1">B3 &amp; ". " &amp; F3</f>
+        <v xml:space="preserve">2. </v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="2">B3</f>
+        <v>2</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J12" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(G3,".",""),"&amp;","")," ","-"),"--","-")</f>
+        <v>2-</v>
+      </c>
+      <c r="M3" t="str">
+        <f>"["&amp;B3&amp;"]"</f>
+        <v>[2]</v>
+      </c>
+      <c r="N3" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B3 &amp; "
+" &amp; M$1 &amp; ": " &amp; M3 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 2
+tags: [2]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">3. </v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="3"/>
+        <v>3-</v>
+      </c>
+      <c r="M4" t="str">
+        <f>"["&amp;B4&amp;"]"</f>
+        <v>[3]</v>
+      </c>
+      <c r="N4" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B4 &amp; "
+" &amp; M$1 &amp; ": " &amp; M4 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 3
+tags: [3]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="3"/>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">4. </v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
+        <v>4-</v>
+      </c>
+      <c r="M5" t="str">
+        <f>"["&amp;B5&amp;"]"</f>
+        <v>[4]</v>
+      </c>
+      <c r="N5" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B5 &amp; "
+" &amp; M$1 &amp; ": " &amp; M5 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 4
+tags: [4]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="3"/>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">5. </v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>5-</v>
+      </c>
+      <c r="M6" t="str">
+        <f>"["&amp;B6&amp;"]"</f>
+        <v>[5]</v>
+      </c>
+      <c r="N6" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B6 &amp; "
+" &amp; M$1 &amp; ": " &amp; M6 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 5
+tags: [5]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">6. </v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>6-</v>
+      </c>
+      <c r="M7" t="str">
+        <f>"["&amp;B7&amp;"]"</f>
+        <v>[6]</v>
+      </c>
+      <c r="N7" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B7 &amp; "
+" &amp; M$1 &amp; ": " &amp; M7 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 6
+tags: [6]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">7. </v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>7-</v>
+      </c>
+      <c r="M8" t="str">
+        <f>"["&amp;B8&amp;"]"</f>
+        <v>[7]</v>
+      </c>
+      <c r="N8" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B8 &amp; "
+" &amp; M$1 &amp; ": " &amp; M8 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 7
+tags: [7]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">8. </v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>8-</v>
+      </c>
+      <c r="M9" t="str">
+        <f>"["&amp;B9&amp;"]"</f>
+        <v>[8]</v>
+      </c>
+      <c r="N9" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B9 &amp; "
+" &amp; M$1 &amp; ": " &amp; M9 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 8
+tags: [8]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">9. </v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>9-</v>
+      </c>
+      <c r="M10" t="str">
+        <f>"["&amp;B10&amp;"]"</f>
+        <v>[9]</v>
+      </c>
+      <c r="N10" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B10 &amp; "
+" &amp; M$1 &amp; ": " &amp; M10 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 9
+tags: [9]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">10. </v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>10-</v>
+      </c>
+      <c r="M11" t="str">
+        <f>"["&amp;B11&amp;"]"</f>
+        <v>[10]</v>
+      </c>
+      <c r="N11" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B11 &amp; "
+" &amp; M$1 &amp; ": " &amp; M11 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 10
+tags: [10]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">11. </v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>11-</v>
+      </c>
+      <c r="M12" t="str">
+        <f>"["&amp;B12&amp;"]"</f>
+        <v>[11]</v>
+      </c>
+      <c r="N12" t="str">
+        <f>"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B12 &amp; "
+" &amp; M$1 &amp; ": " &amp; M12 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 11
+tags: [11]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2">
+        <f t="shared" ref="D13:D15" si="4">IF(LEN(C13),TEXT(C13, "YYYY-MM-DD") &amp; "-" &amp; B13 &amp; ".md",)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G15" si="5">B13 &amp; ". " &amp; F13</f>
+        <v xml:space="preserve">12. </v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H15" si="6">B13</f>
+        <v>12</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ref="J13:J15" si="7">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(G13,".",""),"&amp;","")," ","-"),"--","-")</f>
+        <v>12-</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ref="M13:M15" si="8">"["&amp;B13&amp;"]"</f>
+        <v>[12]</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" ref="N13:N15" si="9">"---
+layout: post
+" &amp; B$1 &amp; ": " &amp; B13 &amp; "
+" &amp; M$1 &amp; ": " &amp; M13 &amp; "
+level: overview
+---"</f>
+        <v>---
+layout: post
+session: 12
+tags: [12]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">13. </v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="7"/>
+        <v>13-</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="8"/>
+        <v>[13]</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="9"/>
+        <v>---
+layout: post
+session: 13
+tags: [13]
+level: overview
+---</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">14. </v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="7"/>
+        <v>14-</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="8"/>
+        <v>[14]</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="9"/>
+        <v>---
+layout: post
+session: 14
+tags: [14]
+level: overview
+---</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added overview photos & session info
</commit_message>
<xml_diff>
--- a/_data/sessions.xlsx
+++ b/_data/sessions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Github/jirelations/24data/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A3DC5-D527-3843-B644-86C138A2F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B5A71B-3B84-BB4D-BDAD-214BDB23BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sessions" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>blank</t>
   </si>
@@ -431,6 +431,51 @@
   </si>
   <si>
     <t>Presentations</t>
+  </si>
+  <si>
+    <t>chocolate-keyboard.png</t>
+  </si>
+  <si>
+    <t>printing-types.jpg</t>
+  </si>
+  <si>
+    <t>vw-beetles.png</t>
+  </si>
+  <si>
+    <t>tables.png</t>
+  </si>
+  <si>
+    <t>refrigerator.png</t>
+  </si>
+  <si>
+    <t>python.png</t>
+  </si>
+  <si>
+    <t>scale.png</t>
+  </si>
+  <si>
+    <t>city-in-hand.png</t>
+  </si>
+  <si>
+    <t>robot.png</t>
+  </si>
+  <si>
+    <t>girl-projector.png</t>
+  </si>
+  <si>
+    <t>photos-conveyor.png</t>
+  </si>
+  <si>
+    <t>breakdance.png</t>
+  </si>
+  <si>
+    <t>baby-chocolate.png</t>
+  </si>
+  <si>
+    <t>droid-camera.png</t>
+  </si>
+  <si>
+    <t>[unicodeinc.WhatUnicode2017, UnicodeCharacterTable2024]</t>
   </si>
 </sst>
 </file>
@@ -442,7 +487,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +528,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -511,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -536,6 +588,7 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +897,8 @@
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -941,12 +994,15 @@
         <v>36</v>
       </c>
       <c r="I2" t="str">
-        <f>B2 &amp; ". " &amp; E2 &amp; ": " &amp; F2</f>
-        <v>1. Introduction: Chocolate</v>
+        <f>B2 &amp; ". " &amp; E2 &amp; ": " &amp; G2</f>
+        <v>1. Introduction: Make Chocolate and Unwrap Your Sources</v>
       </c>
       <c r="J2" s="3">
         <f t="shared" ref="J2:J15" si="1">B2</f>
         <v>1</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="L2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2 &amp; ". " &amp; F2,".",""),"&amp;","")," ","-"),"--","-")</f>
@@ -995,16 +1051,22 @@
         <v>39</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I15" si="3">B3 &amp; ". " &amp; E3 &amp; ": " &amp; F3</f>
-        <v>2. Working with Text: Text</v>
+        <f t="shared" ref="I3:I15" si="3">B3 &amp; ". " &amp; E3 &amp; ": " &amp; G3</f>
+        <v>2. Working with Text: Get the Most out of "Plain" Text and Regular Expressions</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="K3" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L15" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3 &amp; ". " &amp; F3,".",""),"&amp;","")," ","-"),"--","-")</f>
         <v>2-Text</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" si="2"/>
@@ -1050,11 +1112,14 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="3"/>
-        <v>3. Working with Text: Git</v>
+        <v>3. Working with Text: Git Versioning and Archiving Your Data</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="4"/>
@@ -1099,11 +1164,14 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="3"/>
-        <v>4. Working with Text: Markdown &amp; Markup</v>
+        <v>4. Working with Text: Mark it down and Mark it up (HTML and XML)</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="4"/>
@@ -1148,11 +1216,14 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="3"/>
-        <v>5. Accessing &amp; Structuring Datasets: Tables</v>
+        <v>5. Accessing &amp; Structuring Datasets: Structure Your Data with Tables and Databases</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="4"/>
@@ -1197,11 +1268,14 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="3"/>
-        <v>6. Accessing &amp; Structuring Datasets: OpenRefine</v>
+        <v>6. Accessing &amp; Structuring Datasets: Clean and Augment Your Data with OpenRefine</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="4"/>
@@ -1246,11 +1320,14 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="3"/>
-        <v>7. Accessing &amp; Structuring Datasets: Code</v>
+        <v>7. Accessing &amp; Structuring Datasets: Don't Freak out When You See Code (It's Only Python!)</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="1"/>
         <v>7</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="4"/>
@@ -1295,11 +1372,14 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="3"/>
-        <v>8. Accessing &amp; Structuring Datasets: Scraping</v>
+        <v xml:space="preserve">8. Accessing &amp; Structuring Datasets: Grab More Data with Scraping and Querying </v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="4"/>
@@ -1344,11 +1424,14 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="3"/>
-        <v>9. Accessing &amp; Structuring Datasets: FAIR Data</v>
+        <v>9. Accessing &amp; Structuring Datasets: Go Meta with "FAIR" Principles</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="4"/>
@@ -1393,11 +1476,14 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="3"/>
-        <v>10. Advanced Processing &amp; AI: Big Data</v>
+        <v>10. Advanced Processing &amp; AI: Get a Grip on Big Data</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="4"/>
@@ -1442,11 +1528,14 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="3"/>
-        <v>11. Advanced Processing &amp; AI: Images</v>
+        <v>11. Advanced Processing &amp; AI: Process Images and Recognize Text</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="1"/>
         <v>11</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="4"/>
@@ -1491,11 +1580,14 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="3"/>
-        <v>12. Advanced Processing &amp; AI: Audio &amp; Video</v>
+        <v>12. Advanced Processing &amp; AI: Generate and Transcribe Audio and Video</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="4"/>
@@ -1540,11 +1632,14 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="3"/>
-        <v>13. Advanced Processing &amp; AI: AI Labeling</v>
+        <v>13. Advanced Processing &amp; AI: Use AI to Label Your Data</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="4"/>
@@ -1586,11 +1681,14 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="3"/>
-        <v>14. Conclusion: Presentations</v>
+        <v>14. Conclusion: Present Your Dataset</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="4"/>

</xml_diff>